<commit_message>
Updated BOM XLSX and added BOM to README.md.
</commit_message>
<xml_diff>
--- a/homebrew_cpu_BOM.xlsx
+++ b/homebrew_cpu_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\prj\yt\ian_ward\homebrew_cpu\Homebrew-CPU-PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421FBDB8-D457-4157-B151-5FC5F5FF65CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0E0F39-45F8-4E0D-9AE5-1EE337C88CE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="13952" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -296,9 +296,6 @@
     <t>Jameco\2276439</t>
   </si>
   <si>
-    <t>Catalytic capacitor</t>
-  </si>
-  <si>
     <t>Generic</t>
   </si>
   <si>
@@ -471,6 +468,9 @@
   </si>
   <si>
     <t>1Kohm</t>
+  </si>
+  <si>
+    <t>Electrolytic capacitor</t>
   </si>
 </sst>
 </file>
@@ -1387,8 +1387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15C382D7-551C-4DB5-967D-4304CEB98B2E}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.6" x14ac:dyDescent="0.2"/>
@@ -1445,16 +1445,18 @@
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>88</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
       <c r="I2" s="6" t="s">
-        <v>87</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -1505,10 +1507,10 @@
         <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1529,10 +1531,10 @@
         <v>10</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -1553,10 +1555,10 @@
         <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -1565,7 +1567,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C7" s="5">
         <v>2</v>
@@ -1577,16 +1579,16 @@
         <v>61</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="I7" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -1607,16 +1609,16 @@
         <v>62</v>
       </c>
       <c r="F8" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="I8" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -1637,10 +1639,10 @@
         <v>10</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -1661,10 +1663,10 @@
         <v>20</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -1685,16 +1687,16 @@
         <v>69</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="G11" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>95</v>
-      </c>
       <c r="I11" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -1709,22 +1711,22 @@
         <v>3</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -1739,22 +1741,22 @@
         <v>4</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G13" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>141</v>
-      </c>
       <c r="I13" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1769,16 +1771,16 @@
         <v>1</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -1793,16 +1795,16 @@
         <v>1</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -1817,22 +1819,22 @@
         <v>2</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -1847,22 +1849,22 @@
         <v>3</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>29</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="G17" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="H17" s="7" t="s">
+      <c r="H17" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="I17" s="7" t="s">
-        <v>116</v>
+      <c r="I17" s="2" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -1877,7 +1879,7 @@
         <v>1</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>31</v>
@@ -1885,14 +1887,14 @@
       <c r="F18" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="G18" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="H18" s="7" t="s">
+      <c r="H18" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="I18" s="7" t="s">
-        <v>115</v>
+      <c r="I18" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -1913,16 +1915,16 @@
         <v>33</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="G19" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="H19" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="I19" s="7" t="s">
-        <v>114</v>
+      <c r="I19" s="2" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -1943,16 +1945,16 @@
         <v>36</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G20" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H20" s="7" t="s">
+      <c r="H20" s="2" t="s">
         <v>81</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -1973,16 +1975,16 @@
         <v>36</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G21" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H21" s="7" t="s">
+      <c r="H21" s="2" t="s">
         <v>81</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -2003,16 +2005,16 @@
         <v>41</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G22" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H22" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="I22" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -2033,16 +2035,16 @@
         <v>44</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="G23" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H23" s="7" t="s">
+      <c r="H23" s="2" t="s">
         <v>82</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -2063,16 +2065,16 @@
         <v>47</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="G24" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="H24" s="7" t="s">
+      <c r="H24" s="2" t="s">
         <v>83</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -2093,16 +2095,16 @@
         <v>50</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="G25" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="G25" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="H25" s="7" t="s">
+      <c r="H25" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="I25" s="7" t="s">
-        <v>110</v>
+      <c r="I25" s="2" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -2123,16 +2125,16 @@
         <v>53</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="G26" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H26" s="7" t="s">
+      <c r="H26" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="I26" s="7" t="s">
-        <v>109</v>
+      <c r="I26" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>